<commit_message>
Stage 1 of cleanup before integrating into ProjectPenguin
</commit_message>
<xml_diff>
--- a/22.05 pipe diameter finder/input files/Mech GRP foundation for VLS_CUE rev1.xlsx
+++ b/22.05 pipe diameter finder/input files/Mech GRP foundation for VLS_CUE rev1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/104092_grundfos_com/Documents/Documents/git/grundfos-express-tools/pipe diameter finder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/104092_grundfos_com/Documents/Documents/20-29 Areas/22 grundfos-express-tools/22.05 pipe diameter finder/input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{296D9425-ABA9-4914-B13B-89E0BBCBBFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{296D9425-ABA9-4914-B13B-89E0BBCBBFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45127BA0-FAD0-43C7-81A3-D3E9D61AB263}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2235" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GES_VLS_CUE" sheetId="1" r:id="rId1"/>
@@ -71959,7 +71959,7 @@
   <dimension ref="A1:Q1331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72037,6 +72037,9 @@
       <c r="A4" s="1">
         <v>146.73411679742901</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
       <c r="D4" s="1">
         <v>293.46823359485802</v>
       </c>

</xml_diff>